<commit_message>
SQL updated for DSR
</commit_message>
<xml_diff>
--- a/ClientFiles/EMS FLASH SALE DATA ENTRY MODULE V1.xlsx
+++ b/ClientFiles/EMS FLASH SALE DATA ENTRY MODULE V1.xlsx
@@ -5,22 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emine\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Bellona\BellonaUtilities\Bellona\ClientFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D0D02-08FB-4CF5-92BE-A66D5DF5A494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76764D5-9EA5-4364-A797-5DFE39D7B831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D0D9CED-AAF2-4F18-AE28-38A05A293DD9}"/>
   </bookViews>
   <sheets>
-    <sheet name="DSR" sheetId="1" r:id="rId1"/>
-    <sheet name="SALES BUDGET" sheetId="5" r:id="rId2"/>
-    <sheet name="STOCK SHEET" sheetId="2" r:id="rId3"/>
-    <sheet name="MONTHLY EXPENSE" sheetId="3" r:id="rId4"/>
-    <sheet name="DASHBOARD" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="DSR" sheetId="1" r:id="rId2"/>
+    <sheet name="SALES BUDGET" sheetId="5" r:id="rId3"/>
+    <sheet name="STOCK SHEET" sheetId="2" r:id="rId4"/>
+    <sheet name="MONTHLY EXPENSE" sheetId="3" r:id="rId5"/>
+    <sheet name="DASHBOARD" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'MONTHLY EXPENSE'!$B$3:$E$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'MONTHLY EXPENSE'!$B$3:$E$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="240">
   <si>
     <t>FOOD SALE</t>
   </si>
@@ -528,13 +530,251 @@
   </si>
   <si>
     <t>COST HEADS - ( OPTION OF VIEW AND VIEW PLUS EDIT. )</t>
+  </si>
+  <si>
+    <t>Why do we need this?</t>
+  </si>
+  <si>
+    <t>For invoice we have person count, we can directly capture DINE in cover from thr, why do we need to minus from delivery bills?</t>
+  </si>
+  <si>
+    <t>same we can take all sales which are not for delivery then why do we need to minus from delivery sale?</t>
+  </si>
+  <si>
+    <t>Channels</t>
+  </si>
+  <si>
+    <t>Swiggy_Ishaara</t>
+  </si>
+  <si>
+    <t>Takeaway_Eight</t>
+  </si>
+  <si>
+    <t>Zomato_Julius</t>
+  </si>
+  <si>
+    <t>Dine-in_Legume</t>
+  </si>
+  <si>
+    <t>Dinein_Ishaara</t>
+  </si>
+  <si>
+    <t>DotPe-Cha</t>
+  </si>
+  <si>
+    <t>DotPe-Poult</t>
+  </si>
+  <si>
+    <t>Zomato_HOD</t>
+  </si>
+  <si>
+    <t>Zomato_Cha</t>
+  </si>
+  <si>
+    <t>Magicpin-Poult</t>
+  </si>
+  <si>
+    <t>Dine-in_Fyole</t>
+  </si>
+  <si>
+    <t>Swiggy_Legume</t>
+  </si>
+  <si>
+    <t>Magicpin-Caffe Allora</t>
+  </si>
+  <si>
+    <t>Zomato_Ishaara</t>
+  </si>
+  <si>
+    <t>Zomato_Caffe Allora</t>
+  </si>
+  <si>
+    <t>Magicpin-Dobaraa</t>
+  </si>
+  <si>
+    <t>Zomato_Poult</t>
+  </si>
+  <si>
+    <t>Takeaway_Julius</t>
+  </si>
+  <si>
+    <t>Takeaway_Ishaara</t>
+  </si>
+  <si>
+    <t>Takeaway_Poult</t>
+  </si>
+  <si>
+    <t>Delivery_Eight</t>
+  </si>
+  <si>
+    <t>Thrive - Cha</t>
+  </si>
+  <si>
+    <t>Zomato_Eight</t>
+  </si>
+  <si>
+    <t>Dine-in_Cha</t>
+  </si>
+  <si>
+    <t>Swiggy_Eight</t>
+  </si>
+  <si>
+    <t>Dotpe_Dobaara</t>
+  </si>
+  <si>
+    <t>Dine-in_Caffe Allora</t>
+  </si>
+  <si>
+    <t>Swiggy_Poult</t>
+  </si>
+  <si>
+    <t>Swiggy_Cha</t>
+  </si>
+  <si>
+    <t>Swiggy_HOD</t>
+  </si>
+  <si>
+    <t>Takeaway_Caffe Allora</t>
+  </si>
+  <si>
+    <t>Dinein_Dobaara</t>
+  </si>
+  <si>
+    <t>Zomato_Legume</t>
+  </si>
+  <si>
+    <t>Dine-in_Poult</t>
+  </si>
+  <si>
+    <t>Takeaway_Dobaara</t>
+  </si>
+  <si>
+    <t>Dine-in_Julius</t>
+  </si>
+  <si>
+    <t>Swiggy_Fyole</t>
+  </si>
+  <si>
+    <t>Thrive - Ishaara</t>
+  </si>
+  <si>
+    <t>Magicpin-Cha</t>
+  </si>
+  <si>
+    <t>DotPe_Eight</t>
+  </si>
+  <si>
+    <t>Magicpin-Ishaara</t>
+  </si>
+  <si>
+    <t>DotPe-Allora</t>
+  </si>
+  <si>
+    <t>Zomato_Dobaara</t>
+  </si>
+  <si>
+    <t>Dotpe_Fyole</t>
+  </si>
+  <si>
+    <t>Takeaway_Cha</t>
+  </si>
+  <si>
+    <t>Swiggy_Caffe Allora</t>
+  </si>
+  <si>
+    <t>Takeaway_Legume</t>
+  </si>
+  <si>
+    <t>Swiggy_Julius</t>
+  </si>
+  <si>
+    <t>Zomato_Fyole</t>
+  </si>
+  <si>
+    <t>Dinein_Eight</t>
+  </si>
+  <si>
+    <t>Takeaway_Fyole</t>
+  </si>
+  <si>
+    <t>Swiggy_Dobaara</t>
+  </si>
+  <si>
+    <t>Swiggy_Allora Pizzeria</t>
+  </si>
+  <si>
+    <t>Fulfillment Status</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Return_Failed</t>
+  </si>
+  <si>
+    <t>Dispatched</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Processed</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>InvoiceType</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Merged</t>
+  </si>
+  <si>
+    <t>Voided</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>There are multiple invoices which has Dine_in and Delivery both, how to handle them?
+Delivery invoice = 1207 (2024-08-18 23:25:39.0000000 +05:30)
+Pickup = 1271 (2024-08-18 14:36:59.0000000 +05:30)
+How to handle Pickup &amp; Takeaway calculation?
+What about Cancelled &amp; Voided status?</t>
+  </si>
+  <si>
+    <t>No data in system</t>
+  </si>
+  <si>
+    <t>just 3 entry</t>
+  </si>
+  <si>
+    <t>No data in system instead we see Dotpe provider &amp; Magicpin..</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,6 +809,13 @@
       <sz val="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -606,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -618,6 +865,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,84 +1203,449 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231AF830-B921-4901-BCAB-AAF273CD6E88}">
+  <dimension ref="B1:H54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" t="s">
+        <v>223</v>
+      </c>
+      <c r="H6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:H1" xr:uid="{231AF830-B921-4901-BCAB-AAF273CD6E88}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H54">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0714C9B3-082E-4A22-9FB4-6DC8EFB379D7}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A8"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="133.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D14" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D16" s="7" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1076,6 +1692,9 @@
       <c r="A26" t="s">
         <v>136</v>
       </c>
+      <c r="D26" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1096,6 +1715,9 @@
       <c r="A31" t="s">
         <v>140</v>
       </c>
+      <c r="D31" s="6" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1169,6 +1791,9 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>144</v>
+      </c>
+      <c r="D36" t="s">
+        <v>237</v>
       </c>
       <c r="G36">
         <v>189</v>
@@ -1334,7 +1959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7302B5-7D72-4CC3-B2AE-3C5FAD854037}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1415,7 +2040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C452757-CA35-490A-B62A-1E5A92559A78}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -1498,7 +2123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EDC0B5-61EB-4A20-836A-C6FBFB262D4E}">
   <dimension ref="A1:E80"/>
   <sheetViews>
@@ -2543,7 +3168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEA5BBE-83EF-4884-AC46-F611F28FA5E8}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
code change for TB file upload program
</commit_message>
<xml_diff>
--- a/ClientFiles/EMS FLASH SALE DATA ENTRY MODULE V1.xlsx
+++ b/ClientFiles/EMS FLASH SALE DATA ENTRY MODULE V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Bellona\BellonaUtilities\Bellona\ClientFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76764D5-9EA5-4364-A797-5DFE39D7B831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411608CB-C3AD-46F5-A692-E6507DE60AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D0D9CED-AAF2-4F18-AE28-38A05A293DD9}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="264">
   <si>
     <t>FOOD SALE</t>
   </si>
@@ -530,9 +530,6 @@
   </si>
   <si>
     <t>COST HEADS - ( OPTION OF VIEW AND VIEW PLUS EDIT. )</t>
-  </si>
-  <si>
-    <t>Why do we need this?</t>
   </si>
   <si>
     <t>For invoice we have person count, we can directly capture DINE in cover from thr, why do we need to minus from delivery bills?</t>
@@ -769,12 +766,87 @@
   <si>
     <t>No data in system instead we see Dotpe provider &amp; Magicpin..</t>
   </si>
+  <si>
+    <t>How to get it?</t>
+  </si>
+  <si>
+    <t>Easy Diner</t>
+  </si>
+  <si>
+    <t>Gpay</t>
+  </si>
+  <si>
+    <t>dotpe googlepay</t>
+  </si>
+  <si>
+    <t>Dineout</t>
+  </si>
+  <si>
+    <t>UPI Payment</t>
+  </si>
+  <si>
+    <t>dotpe paytm</t>
+  </si>
+  <si>
+    <t>Paytm Deals</t>
+  </si>
+  <si>
+    <t>Zomato</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>magicpin</t>
+  </si>
+  <si>
+    <t>dotpe phonepe</t>
+  </si>
+  <si>
+    <t>dotpe debitCard</t>
+  </si>
+  <si>
+    <t>Zomato Pro</t>
+  </si>
+  <si>
+    <t>BOOK MY SHOW</t>
+  </si>
+  <si>
+    <t>SWIGGY Dineout</t>
+  </si>
+  <si>
+    <t>Cash Sales</t>
+  </si>
+  <si>
+    <t>dotpe simpl</t>
+  </si>
+  <si>
+    <t>Credit Card Sales</t>
+  </si>
+  <si>
+    <t>Thrive</t>
+  </si>
+  <si>
+    <t>Sodexo</t>
+  </si>
+  <si>
+    <t>PAYTM</t>
+  </si>
+  <si>
+    <t>dotpe creditCard</t>
+  </si>
+  <si>
+    <t>Swiggy</t>
+  </si>
+  <si>
+    <t>Payment Mode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1204,339 +1276,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231AF830-B921-4901-BCAB-AAF273CD6E88}">
-  <dimension ref="B1:H54"/>
+  <dimension ref="B1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.09765625" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.19921875" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10">
       <c r="B1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10">
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H3" t="s">
+        <v>232</v>
+      </c>
+      <c r="J3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>220</v>
+      </c>
+      <c r="H4" t="s">
+        <v>230</v>
+      </c>
+      <c r="J4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" t="s">
+        <v>225</v>
+      </c>
+      <c r="H5" t="s">
+        <v>233</v>
+      </c>
+      <c r="J5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" t="s">
+        <v>231</v>
+      </c>
+      <c r="J6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" t="s">
+        <v>224</v>
+      </c>
+      <c r="J7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" t="s">
+        <v>221</v>
+      </c>
+      <c r="J8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>200</v>
+      </c>
+      <c r="J9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+      <c r="J11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+      <c r="J12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>204</v>
+      </c>
+      <c r="J13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
+        <v>208</v>
+      </c>
+      <c r="J14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" t="s">
+        <v>206</v>
+      </c>
+      <c r="J15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" t="s">
+        <v>203</v>
+      </c>
+      <c r="J19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" t="s">
+        <v>180</v>
+      </c>
+      <c r="J20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" t="s">
+        <v>205</v>
+      </c>
+      <c r="J21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" t="s">
+        <v>174</v>
+      </c>
+      <c r="J22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" t="s">
+        <v>217</v>
+      </c>
+      <c r="J23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" t="s">
+        <v>210</v>
+      </c>
+      <c r="J24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
         <v>186</v>
       </c>
-      <c r="D2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F2" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F3" t="s">
-        <v>229</v>
-      </c>
-      <c r="H3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" t="s">
-        <v>221</v>
-      </c>
-      <c r="H4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
         <v>197</v>
       </c>
-      <c r="D5" t="s">
-        <v>226</v>
-      </c>
-      <c r="H5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D6" t="s">
-        <v>223</v>
-      </c>
-      <c r="H6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1553,173 +1698,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0714C9B3-082E-4A22-9FB4-6DC8EFB379D7}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="133.33203125" customWidth="1"/>
+    <col min="1" max="1" width="50.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.8984375" customWidth="1"/>
+    <col min="3" max="3" width="1.5" customWidth="1"/>
+    <col min="4" max="4" width="133.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="21" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>162</v>
+        <v>239</v>
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>152</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="96.6">
       <c r="D16" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>136</v>
       </c>
       <c r="D26" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>140</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>141</v>
       </c>
@@ -1737,7 +1884,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>142</v>
       </c>
@@ -1755,7 +1902,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -1773,7 +1920,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="G35">
         <v>392</v>
       </c>
@@ -1788,12 +1935,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>144</v>
       </c>
       <c r="D36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G36">
         <v>189</v>
@@ -1809,7 +1956,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -1827,7 +1974,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>146</v>
       </c>
@@ -1842,7 +1989,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -1857,7 +2004,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="G40">
         <v>336</v>
       </c>
@@ -1869,7 +2016,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -1884,7 +2031,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -1899,7 +2046,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>150</v>
       </c>
@@ -1914,7 +2061,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>151</v>
       </c>
@@ -1929,7 +2076,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="G45">
         <v>196</v>
       </c>
@@ -1941,7 +2088,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="G46">
         <v>392</v>
       </c>
@@ -1967,52 +2114,52 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2020,17 +2167,17 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -2048,20 +2195,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.19921875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" customWidth="1"/>
+    <col min="7" max="7" width="23.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -2093,27 +2240,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2131,19 +2278,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="B3" s="3" t="s">
         <v>31</v>
       </c>
@@ -2157,7 +2304,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="B4" s="3" t="s">
         <v>131</v>
       </c>
@@ -2171,7 +2318,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
@@ -2185,7 +2332,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
@@ -2199,7 +2346,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
@@ -2213,7 +2360,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2227,7 +2374,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -2241,7 +2388,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
@@ -2255,7 +2402,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
@@ -2269,7 +2416,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
@@ -2283,7 +2430,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="B13" s="3" t="s">
         <v>132</v>
       </c>
@@ -2295,7 +2442,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
@@ -2309,7 +2456,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
@@ -2323,7 +2470,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
@@ -2337,7 +2484,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
@@ -2351,7 +2498,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
@@ -2365,7 +2512,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
@@ -2379,7 +2526,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
@@ -2393,7 +2540,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
@@ -2407,7 +2554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
@@ -2421,7 +2568,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
@@ -2435,7 +2582,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3" t="s">
         <v>56</v>
       </c>
@@ -2449,7 +2596,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
@@ -2463,7 +2610,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="B26" s="3" t="s">
         <v>59</v>
       </c>
@@ -2477,7 +2624,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
@@ -2491,7 +2638,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5">
       <c r="B28" s="3" t="s">
         <v>62</v>
       </c>
@@ -2505,7 +2652,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5">
       <c r="B29" s="3" t="s">
         <v>64</v>
       </c>
@@ -2519,7 +2666,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5">
       <c r="B30" s="3" t="s">
         <v>65</v>
       </c>
@@ -2533,7 +2680,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5">
       <c r="B31" s="3" t="s">
         <v>66</v>
       </c>
@@ -2547,7 +2694,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5">
       <c r="B32" s="3" t="s">
         <v>68</v>
       </c>
@@ -2561,7 +2708,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5">
       <c r="B33" s="3" t="s">
         <v>69</v>
       </c>
@@ -2575,7 +2722,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5">
       <c r="B34" s="3" t="s">
         <v>70</v>
       </c>
@@ -2589,7 +2736,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5">
       <c r="B35" s="3" t="s">
         <v>71</v>
       </c>
@@ -2603,7 +2750,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5">
       <c r="B36" s="3" t="s">
         <v>72</v>
       </c>
@@ -2617,7 +2764,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5">
       <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
@@ -2631,7 +2778,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5">
       <c r="B38" s="3" t="s">
         <v>74</v>
       </c>
@@ -2645,7 +2792,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5">
       <c r="B39" s="3" t="s">
         <v>76</v>
       </c>
@@ -2659,7 +2806,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5">
       <c r="B40" s="3" t="s">
         <v>77</v>
       </c>
@@ -2673,7 +2820,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5">
       <c r="B41" s="3" t="s">
         <v>78</v>
       </c>
@@ -2687,7 +2834,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5">
       <c r="B42" s="3" t="s">
         <v>80</v>
       </c>
@@ -2701,7 +2848,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5">
       <c r="B43" s="3" t="s">
         <v>82</v>
       </c>
@@ -2715,7 +2862,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5">
       <c r="B44" s="3" t="s">
         <v>83</v>
       </c>
@@ -2729,7 +2876,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5">
       <c r="B45" s="3" t="s">
         <v>84</v>
       </c>
@@ -2743,7 +2890,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5">
       <c r="B46" s="3" t="s">
         <v>86</v>
       </c>
@@ -2757,7 +2904,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5">
       <c r="B47" s="3" t="s">
         <v>87</v>
       </c>
@@ -2771,7 +2918,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5">
       <c r="B48" s="3" t="s">
         <v>88</v>
       </c>
@@ -2785,7 +2932,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5">
       <c r="B49" s="3" t="s">
         <v>89</v>
       </c>
@@ -2799,7 +2946,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5">
       <c r="B50" s="3" t="s">
         <v>90</v>
       </c>
@@ -2813,7 +2960,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5">
       <c r="B51" s="3" t="s">
         <v>91</v>
       </c>
@@ -2827,7 +2974,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5">
       <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
@@ -2841,7 +2988,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5">
       <c r="B53" s="3" t="s">
         <v>124</v>
       </c>
@@ -2855,7 +3002,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5">
       <c r="B54" s="3" t="s">
         <v>125</v>
       </c>
@@ -2869,7 +3016,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5">
       <c r="B55" s="3" t="s">
         <v>93</v>
       </c>
@@ -2883,7 +3030,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5">
       <c r="B56" s="3" t="s">
         <v>95</v>
       </c>
@@ -2897,7 +3044,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
@@ -2905,7 +3052,7 @@
       </c>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5">
       <c r="B58" s="3" t="s">
         <v>96</v>
       </c>
@@ -2919,7 +3066,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5">
       <c r="B59" s="3" t="s">
         <v>97</v>
       </c>
@@ -2933,7 +3080,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5">
       <c r="B60" s="3" t="s">
         <v>99</v>
       </c>
@@ -2947,7 +3094,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5">
       <c r="B61" s="3" t="s">
         <v>100</v>
       </c>
@@ -2961,7 +3108,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5">
       <c r="B62" s="3" t="s">
         <v>102</v>
       </c>
@@ -2975,7 +3122,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5">
       <c r="B63" s="3" t="s">
         <v>103</v>
       </c>
@@ -2989,7 +3136,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5">
       <c r="B64" s="3" t="s">
         <v>104</v>
       </c>
@@ -3003,7 +3150,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5">
       <c r="B65" s="3" t="s">
         <v>107</v>
       </c>
@@ -3017,7 +3164,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5">
       <c r="B66" s="3" t="s">
         <v>108</v>
       </c>
@@ -3031,7 +3178,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5">
       <c r="B67" s="3" t="s">
         <v>109</v>
       </c>
@@ -3045,7 +3192,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5">
       <c r="B68" s="3" t="s">
         <v>110</v>
       </c>
@@ -3059,7 +3206,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5">
       <c r="B69" s="3" t="s">
         <v>112</v>
       </c>
@@ -3073,7 +3220,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5">
       <c r="B70" s="3" t="s">
         <v>113</v>
       </c>
@@ -3087,7 +3234,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5">
       <c r="B71" s="3" t="s">
         <v>114</v>
       </c>
@@ -3101,7 +3248,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5">
       <c r="B72" s="5" t="s">
         <v>116</v>
       </c>
@@ -3115,42 +3262,42 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5">
       <c r="B74" s="4"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5">
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5">
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5">
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5">
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5">
       <c r="B79" s="4"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5">
       <c r="B80" s="5" t="s">
         <v>116</v>
       </c>
@@ -3176,9 +3323,9 @@
       <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>